<commit_message>
added support for I2C EEPROM
</commit_message>
<xml_diff>
--- a/sfw/U1101_firmware/Microcontroller_Peripheral_Map.xlsx
+++ b/sfw/U1101_firmware/Microcontroller_Peripheral_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\LED_Panel_Controller\sfw\U1101_firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48798BE9-D0FC-48A6-9537-D4FE00522CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB4EA5D-D82B-4666-83CF-3107E55B3B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3540" windowWidth="24240" windowHeight="13740" xr2:uid="{B7D91EF5-14DE-4003-8C97-5F77E28EC198}"/>
   </bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>